<commit_message>
Added CID field, expanded example text
</commit_message>
<xml_diff>
--- a/xlspy.xlsx
+++ b/xlspy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Compound</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t xml:space="preserve">C8H8O2
+</t>
+  </si>
+  <si>
+    <t>Remdesivir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-ethylbutyl (2S)-2-[[[(2R,3S,4R,5R)-5-(4-aminopyrrolo[2,1-f][1,2,4]triazin-7-yl)-5-cyano-3,4-dihydroxyoxolan-2-yl]methoxy-phenoxyphosphoryl]amino]propanoate
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">602.6
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27H35N6O8P
 </t>
   </si>
 </sst>
@@ -390,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,6 +432,9 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2">
+        <v>2776299</v>
+      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -431,6 +449,9 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3">
+        <v>999</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -439,6 +460,23 @@
       </c>
       <c r="E3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>121304016</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added blank line check
</commit_message>
<xml_diff>
--- a/xlspy.xlsx
+++ b/xlspy.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Compound</t>
   </si>
@@ -74,6 +74,9 @@
   <si>
     <t xml:space="preserve">C27H35N6O8P
 </t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -479,6 +482,34 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>